<commit_message>
Added a date support for excel parser in multivisualisation module. Resolved #791
</commit_message>
<xml_diff>
--- a/abixen-platform-business-intelligence-service/src/test/resource/excelCorrect.xlsx
+++ b/abixen-platform-business-intelligence-service/src/test/resource/excelCorrect.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Col1</t>
   </si>
@@ -25,6 +25,9 @@
   </si>
   <si>
     <t>Col3</t>
+  </si>
+  <si>
+    <t>Col4</t>
   </si>
 </sst>
 </file>
@@ -61,8 +64,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -357,15 +361,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D1" sqref="D1:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -375,8 +382,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -386,8 +396,11 @@
       <c r="C2">
         <v>333</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="1">
+        <v>41779</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -397,8 +410,11 @@
       <c r="C3">
         <v>334</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="1">
+        <v>41780</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -408,8 +424,11 @@
       <c r="C4">
         <v>335</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="1">
+        <v>41781</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -419,8 +438,11 @@
       <c r="C5">
         <v>336</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" s="1">
+        <v>41782</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -430,8 +452,11 @@
       <c r="C6">
         <v>337</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" s="1">
+        <v>41783</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>6</v>
       </c>
@@ -441,8 +466,11 @@
       <c r="C7">
         <v>338</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" s="1">
+        <v>41784</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>7</v>
       </c>
@@ -452,8 +480,11 @@
       <c r="C8">
         <v>339</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" s="1">
+        <v>41785</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>8</v>
       </c>
@@ -463,8 +494,11 @@
       <c r="C9">
         <v>340</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" s="1">
+        <v>41786</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>9</v>
       </c>
@@ -474,8 +508,11 @@
       <c r="C10">
         <v>341</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" s="1">
+        <v>41787</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>10</v>
       </c>
@@ -485,8 +522,11 @@
       <c r="C11">
         <v>342</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" s="1">
+        <v>41788</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>11</v>
       </c>
@@ -496,8 +536,11 @@
       <c r="C12">
         <v>343</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12" s="1">
+        <v>41789</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>12</v>
       </c>
@@ -507,8 +550,11 @@
       <c r="C13">
         <v>344</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" s="1">
+        <v>41790</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>13</v>
       </c>
@@ -518,8 +564,11 @@
       <c r="C14">
         <v>345</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14" s="1">
+        <v>41791</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>14</v>
       </c>
@@ -529,8 +578,11 @@
       <c r="C15">
         <v>346</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15" s="1">
+        <v>41792</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>15</v>
       </c>
@@ -540,8 +592,11 @@
       <c r="C16">
         <v>347</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" s="1">
+        <v>41793</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>16</v>
       </c>
@@ -551,8 +606,11 @@
       <c r="C17">
         <v>348</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" s="1">
+        <v>41794</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>17</v>
       </c>
@@ -562,8 +620,11 @@
       <c r="C18">
         <v>349</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18" s="1">
+        <v>41795</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>18</v>
       </c>
@@ -573,8 +634,11 @@
       <c r="C19">
         <v>350</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19" s="1">
+        <v>41796</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>19</v>
       </c>
@@ -584,8 +648,11 @@
       <c r="C20">
         <v>351</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20" s="1">
+        <v>41797</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>20</v>
       </c>
@@ -595,10 +662,13 @@
       <c r="C21">
         <v>352</v>
       </c>
+      <c r="D21" s="1">
+        <v>41798</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>